<commit_message>
updated tables and implenntation documents
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/likarajo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/likarajo/Work/GitHub/DallasCare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3EFD5A-588A-2C4A-97F8-5CF903981C8F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14B6160A-F86B-3940-BACD-9BC913021071}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16140" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="16140" windowHeight="16660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -561,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AC12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AD16" sqref="AD16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1:AC8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>